<commit_message>
A and B results
</commit_message>
<xml_diff>
--- a/hiv/datadict/dict.xlsx
+++ b/hiv/datadict/dict.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="70">
   <si>
     <t>study</t>
   </si>
@@ -136,6 +136,105 @@
   </si>
   <si>
     <t>study result publication</t>
+  </si>
+  <si>
+    <t>NCT01165203</t>
+  </si>
+  <si>
+    <t>Dataset Specification</t>
+  </si>
+  <si>
+    <t>https://www.clinicalstudydatarequest.com</t>
+  </si>
+  <si>
+    <t>For additional information about this study please refer to the GSK Clinical Study Register</t>
+  </si>
+  <si>
+    <t>Individual Participant Data Set</t>
+  </si>
+  <si>
+    <t>NCT00933595</t>
+  </si>
+  <si>
+    <t>LUNG-HIV</t>
+  </si>
+  <si>
+    <t>http://biolincc.nhlbi.nih.gov/studies/lung_hiv/</t>
+  </si>
+  <si>
+    <t>NHLBI provides controlled access to IPD through BioLINCC. Access requires registration, evidence of local IRB approval or certification of exemption from IRB review, and completion of a data use agreement.</t>
+  </si>
+  <si>
+    <t>NCT00829010</t>
+  </si>
+  <si>
+    <t>NCT00586339</t>
+  </si>
+  <si>
+    <t>NCT00097006</t>
+  </si>
+  <si>
+    <t>REDS II-CORE</t>
+  </si>
+  <si>
+    <t>http://biolincc.nhlbi.nih.gov/studies/core/</t>
+  </si>
+  <si>
+    <t>REDS II-LAPS</t>
+  </si>
+  <si>
+    <t>http://biolincc.nhlbi.nih.gov/studies/laps/</t>
+  </si>
+  <si>
+    <t>REDS II-MS</t>
+  </si>
+  <si>
+    <t>http://biolincc.nhlbi.nih.gov/studies/redsms/</t>
+  </si>
+  <si>
+    <t>REDS II-RISE</t>
+  </si>
+  <si>
+    <t>http://biolincc.nhlbi.nih.gov/studies/rise/</t>
+  </si>
+  <si>
+    <t>NCT00005278</t>
+  </si>
+  <si>
+    <t>REDS-HTLV</t>
+  </si>
+  <si>
+    <t>http://biolincc.nhlbi.nih.gov/studies/reds/</t>
+  </si>
+  <si>
+    <t>NCT00005274</t>
+  </si>
+  <si>
+    <t>P2C2</t>
+  </si>
+  <si>
+    <t>http://biolincc.nhlbi.nih.gov/studies/p2c2/</t>
+  </si>
+  <si>
+    <t>NCT00000593</t>
+  </si>
+  <si>
+    <t>VATS</t>
+  </si>
+  <si>
+    <t>http://biolincc.nhlbi.nih.gov/studies/vats/</t>
+  </si>
+  <si>
+    <t>NCT00000590</t>
+  </si>
+  <si>
+    <t>PACTG</t>
+  </si>
+  <si>
+    <t>http://biolincc.nhlbi.nih.gov/studies/pactg/</t>
+  </si>
+  <si>
+    <t>ignore</t>
   </si>
 </sst>
 </file>
@@ -453,74 +552,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
       <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
         <v>1</v>
       </c>
@@ -536,41 +633,41 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>32</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0</v>
       </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
         <v>20</v>
       </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
         <v>1</v>
       </c>
@@ -586,41 +683,44 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>31</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
       <c r="N3">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
         <v>20</v>
       </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4">
         <v>1</v>
       </c>
@@ -630,42 +730,407 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>11</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>36</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>32</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
       <c r="N4">
         <v>1</v>
       </c>
-      <c r="P4" t="s">
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
         <v>19</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14">
+        <v>112673</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16">
+        <v>111634</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17">
+        <v>107863</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30">
+        <v>112673</v>
+      </c>
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31">
+        <v>112673</v>
+      </c>
+      <c r="E31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33">
+        <v>111634</v>
+      </c>
+      <c r="E33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34">
+        <v>111634</v>
+      </c>
+      <c r="E34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35">
+        <v>107863</v>
+      </c>
+      <c r="E35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36">
+        <v>107863</v>
+      </c>
+      <c r="E36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" t="s">
+        <v>54</v>
+      </c>
+      <c r="G39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" t="s">
+        <v>41</v>
+      </c>
+      <c r="F42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" t="s">
+        <v>41</v>
+      </c>
+      <c r="F43" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G44" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>